<commit_message>
Finished translating comments Small changes
</commit_message>
<xml_diff>
--- a/input_test.xlsx
+++ b/input_test.xlsx
@@ -10,11 +10,12 @@
   <sheets>
     <sheet name="TestCases" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="TestSheet0" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="EmptySheet" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="EmptySheetEng" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Salvador" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Irgwi-Config" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Irgwi-Allosaurus" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="TestSheet1" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="EmptySheet" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="EmptySheetEng" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Salvador" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Irgwi-Config" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Irgwi-Allosaurus" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,11 +27,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
   <si>
     <t xml:space="preserve">Testfälle</t>
   </si>
   <si>
+    <t xml:space="preserve">1 Angriff, 1 Waffe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unerwünschte Eingaben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leere Eingabedatei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fehlende Angaben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fehlende Zeilen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falsch benannte Zeilen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mehr als eine Leerzeile zwischen Waffen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Schadenswürfel</t>
   </si>
   <si>
@@ -80,6 +102,15 @@
   </si>
   <si>
     <t xml:space="preserve">Schadensreduzierung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-2</t>
   </si>
   <si>
     <t xml:space="preserve">Base Damage Dice</t>
@@ -290,10 +321,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -305,6 +336,41 @@
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -345,7 +411,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -355,7 +421,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -365,7 +431,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -375,7 +441,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -385,7 +451,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -395,7 +461,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -405,7 +471,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -415,7 +481,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -425,7 +491,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -435,7 +501,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -445,7 +511,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -455,7 +521,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -465,7 +531,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -475,7 +541,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -485,7 +551,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -495,7 +561,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -505,7 +571,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -531,7 +597,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -541,7 +607,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -551,7 +617,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -561,7 +627,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -571,7 +637,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -581,7 +647,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -591,7 +657,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -601,7 +667,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -611,7 +677,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -621,7 +687,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -631,7 +697,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -641,7 +707,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -651,7 +717,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -661,7 +727,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -671,7 +737,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -681,7 +747,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -691,7 +757,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -711,6 +777,494 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="26.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="5" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" s="5" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -737,7 +1291,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -747,7 +1301,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -757,7 +1311,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -767,7 +1321,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -777,7 +1331,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -787,7 +1341,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -797,7 +1351,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -807,7 +1361,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -817,7 +1371,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -827,7 +1381,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -837,7 +1391,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -847,7 +1401,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -857,7 +1411,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -867,7 +1421,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -877,7 +1431,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -887,7 +1441,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -897,7 +1451,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -924,7 +1478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -951,7 +1505,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -961,7 +1515,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -971,7 +1525,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -981,7 +1535,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -991,7 +1545,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1001,7 +1555,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1011,7 +1565,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1021,7 +1575,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1031,7 +1585,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1041,7 +1595,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1051,7 +1605,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1061,7 +1615,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1071,7 +1625,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1081,7 +1635,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1091,7 +1645,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1101,7 +1655,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1111,7 +1665,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1138,7 +1692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1146,7 +1700,7 @@
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q17" activeCellId="0" sqref="Q17"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1159,30 +1713,30 @@
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="7" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="Z1" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>1</v>
@@ -1229,7 +1783,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>0</v>
@@ -1297,7 +1851,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>21</v>
@@ -1326,7 +1880,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>25</v>
@@ -1355,7 +1909,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>19</v>
@@ -1383,7 +1937,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>2</v>
@@ -1409,7 +1963,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>0</v>
@@ -1435,7 +1989,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F9" s="6"/>
       <c r="J9" s="6"/>
@@ -1446,7 +2000,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6" t="n">
         <v>0</v>
@@ -1472,7 +2026,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F11" s="6"/>
       <c r="J11" s="6" t="n">
@@ -1503,7 +2057,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F12" s="6"/>
       <c r="J12" s="6"/>
@@ -1519,7 +2073,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6" t="n">
         <v>0</v>
@@ -1545,7 +2099,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>0</v>
@@ -1571,7 +2125,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>0</v>
@@ -1597,7 +2151,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>0</v>
@@ -1623,7 +2177,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>0</v>
@@ -1649,7 +2203,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>0</v>
@@ -1692,7 +2246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1715,7 +2269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1742,7 +2296,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1752,7 +2306,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1762,7 +2316,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1772,7 +2326,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1782,7 +2336,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1792,7 +2346,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1802,7 +2356,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1812,7 +2366,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1822,7 +2376,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1832,7 +2386,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1842,7 +2396,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1852,7 +2406,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1862,7 +2416,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1872,7 +2426,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1882,7 +2436,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1892,7 +2446,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1902,7 +2456,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>

</xml_diff>

<commit_message>
- Created example input file - Implemented main function and args for starting and configuring the program from command line - Implemented Sheet.printData() - Created help text function - Program does no longer print difference matrix with only one attack
</commit_message>
<xml_diff>
--- a/input_test.xlsx
+++ b/input_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,7 @@
     <sheet name="Vanya" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Tannenquelle-Config" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Tannenquelle" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Koboldstein" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -30,12 +31,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="82">
   <si>
     <t xml:space="preserve">Testfälle</t>
   </si>
   <si>
     <t xml:space="preserve">1 Angriff, 1 Waffe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fehlerhaft übergebene Argumente</t>
   </si>
   <si>
     <t xml:space="preserve">Unerwünschte Eingaben</t>
@@ -514,16 +518,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,35 +541,38 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +594,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -601,35 +610,35 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
@@ -644,7 +653,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="n">
         <f aca="false">$B$2+$C$9+$B$3 + SUM($E6:$S6)</f>
@@ -665,7 +674,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="n">
         <f aca="false">$C$9 + SUM($E7:$S7)</f>
@@ -683,7 +692,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>20</v>
@@ -715,7 +724,7 @@
   <dimension ref="A1:AMJ59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
+      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -727,19 +736,19 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -747,19 +756,19 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
@@ -767,7 +776,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>1</v>
@@ -802,7 +811,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>0</v>
@@ -838,7 +847,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
         <f aca="false">'Tannenquelle-Config'!$B$6</f>
@@ -859,7 +868,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="n">
         <f aca="false">'Tannenquelle-Config'!$B$7</f>
@@ -880,7 +889,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>18</v>
@@ -900,7 +909,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>2</v>
@@ -920,7 +929,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>0</v>
@@ -940,12 +949,12 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>0</v>
@@ -965,7 +974,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N12" s="6" t="n">
         <v>1</v>
@@ -976,12 +985,12 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>0</v>
@@ -1001,7 +1010,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>0</v>
@@ -1021,7 +1030,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>0</v>
@@ -1041,7 +1050,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>0</v>
@@ -1061,7 +1070,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>0</v>
@@ -1081,7 +1090,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>5</v>
@@ -1113,6 +1122,252 @@
       <c r="AMH59" s="0"/>
       <c r="AMI59" s="0"/>
       <c r="AMJ59" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="6" width="3.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="62" style="1" width="11.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="20" s="4" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1133,10 +1388,10 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -1160,7 +1415,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1170,7 +1425,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1180,7 +1435,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1190,7 +1445,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1200,7 +1455,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1210,7 +1465,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1220,7 +1475,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1230,7 +1485,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1240,7 +1495,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1250,7 +1505,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1260,7 +1515,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1270,7 +1525,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1280,7 +1535,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1290,7 +1545,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1300,7 +1555,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1310,7 +1565,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1320,7 +1575,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1346,7 +1601,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1356,7 +1611,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1366,7 +1621,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1376,7 +1631,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1386,7 +1641,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1396,7 +1651,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1406,7 +1661,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1416,7 +1671,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1426,7 +1681,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1436,7 +1691,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1446,7 +1701,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1456,7 +1711,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1466,7 +1721,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1476,7 +1731,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1486,7 +1741,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1496,7 +1751,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1506,7 +1761,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1533,10 +1788,10 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -1560,7 +1815,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>0</v>
@@ -1574,7 +1829,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>21</v>
@@ -1588,7 +1843,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>25</v>
@@ -1602,7 +1857,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>19</v>
@@ -1616,7 +1871,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>2</v>
@@ -1630,7 +1885,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>0</v>
@@ -1644,7 +1899,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="1"/>
@@ -1654,7 +1909,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="6" t="n">
         <v>0</v>
@@ -1668,7 +1923,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="1"/>
@@ -1678,7 +1933,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
@@ -1688,7 +1943,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="6" t="n">
         <v>0</v>
@@ -1702,7 +1957,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>0</v>
@@ -1716,7 +1971,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>0</v>
@@ -1730,7 +1985,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>0</v>
@@ -1744,7 +1999,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>0</v>
@@ -1758,7 +2013,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>0</v>
@@ -1788,7 +2043,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>1</v>
@@ -1802,7 +2057,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22" s="6" t="n">
         <v>0</v>
@@ -1814,7 +2069,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B23" s="6" t="n">
         <v>21</v>
@@ -1826,7 +2081,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" s="6" t="n">
         <v>25</v>
@@ -1838,7 +2093,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25" s="6" t="n">
         <v>19</v>
@@ -1850,7 +2105,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B26" s="6" t="n">
         <v>2</v>
@@ -1862,7 +2117,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" s="6" t="n">
         <v>0</v>
@@ -1874,7 +2129,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="1"/>
@@ -1884,7 +2139,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B29" s="6" t="n">
         <v>0</v>
@@ -1896,7 +2151,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="1"/>
@@ -1906,7 +2161,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="1"/>
@@ -1916,7 +2171,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B32" s="6" t="n">
         <v>0</v>
@@ -1928,7 +2183,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B33" s="6" t="n">
         <v>0</v>
@@ -1940,7 +2195,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B34" s="6" t="n">
         <v>0</v>
@@ -1952,7 +2207,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B35" s="6" t="n">
         <v>0</v>
@@ -1964,7 +2219,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B36" s="6" t="n">
         <v>0</v>
@@ -1976,7 +2231,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B37" s="6" t="n">
         <v>0</v>
@@ -2005,10 +2260,10 @@
   <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y42" activeCellId="0" sqref="Y42"/>
+      <selection pane="topLeft" activeCell="Y42" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -2032,7 +2287,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -2042,7 +2297,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>0</v>
@@ -2054,7 +2309,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>0</v>
@@ -2066,7 +2321,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>0</v>
@@ -2078,7 +2333,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>20</v>
@@ -2090,7 +2345,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>2</v>
@@ -2102,7 +2357,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>0</v>
@@ -2114,7 +2369,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2124,7 +2379,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>0</v>
@@ -2136,7 +2391,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -2146,7 +2401,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2156,7 +2411,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>0</v>
@@ -2168,7 +2423,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>0</v>
@@ -2180,7 +2435,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>0</v>
@@ -2192,7 +2447,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>0</v>
@@ -2204,7 +2459,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>0</v>
@@ -2216,7 +2471,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>0</v>
@@ -2244,7 +2499,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -2254,7 +2509,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="6" t="n">
         <v>0</v>
@@ -2266,7 +2521,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B24" s="6" t="n">
         <v>0</v>
@@ -2278,7 +2533,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B25" s="6" t="n">
         <v>0</v>
@@ -2290,7 +2545,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" s="6" t="n">
         <v>20</v>
@@ -2302,7 +2557,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B27" s="6" t="n">
         <v>2</v>
@@ -2314,7 +2569,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B28" s="6" t="n">
         <v>0</v>
@@ -2326,7 +2581,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -2336,7 +2591,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B30" s="6" t="n">
         <v>0</v>
@@ -2348,7 +2603,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -2358,7 +2613,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -2368,7 +2623,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B33" s="6" t="n">
         <v>0</v>
@@ -2380,7 +2635,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B34" s="6" t="n">
         <v>0</v>
@@ -2392,7 +2647,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B35" s="6" t="n">
         <v>0</v>
@@ -2404,7 +2659,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B36" s="6" t="n">
         <v>0</v>
@@ -2416,7 +2671,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B37" s="6" t="n">
         <v>0</v>
@@ -2428,7 +2683,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B38" s="6" t="n">
         <v>0</v>
@@ -2448,7 +2703,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -2458,7 +2713,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B42" s="6" t="n">
         <v>0</v>
@@ -2470,7 +2725,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B43" s="6" t="n">
         <v>0</v>
@@ -2482,7 +2737,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B44" s="6" t="n">
         <v>0</v>
@@ -2494,7 +2749,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B45" s="6" t="n">
         <v>20</v>
@@ -2506,7 +2761,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B46" s="6" t="n">
         <v>2</v>
@@ -2518,7 +2773,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B47" s="6" t="n">
         <v>0</v>
@@ -2530,7 +2785,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -2540,7 +2795,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B49" s="6" t="n">
         <v>0</v>
@@ -2552,7 +2807,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -2562,7 +2817,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -2572,7 +2827,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B52" s="6" t="n">
         <v>0</v>
@@ -2584,7 +2839,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B53" s="6" t="n">
         <v>0</v>
@@ -2596,7 +2851,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B54" s="6" t="n">
         <v>0</v>
@@ -2608,7 +2863,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B55" s="6" t="n">
         <v>0</v>
@@ -2620,7 +2875,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B56" s="6" t="n">
         <v>0</v>
@@ -2632,7 +2887,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B57" s="6" t="n">
         <v>0</v>
@@ -2652,7 +2907,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -2662,7 +2917,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B61" s="6" t="n">
         <v>0</v>
@@ -2674,7 +2929,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B62" s="6" t="n">
         <v>0</v>
@@ -2686,7 +2941,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B63" s="6" t="n">
         <v>0</v>
@@ -2698,7 +2953,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B64" s="6" t="n">
         <v>20</v>
@@ -2710,7 +2965,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B65" s="6" t="n">
         <v>2</v>
@@ -2722,7 +2977,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B66" s="6" t="n">
         <v>0</v>
@@ -2734,7 +2989,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -2744,7 +2999,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B68" s="6" t="n">
         <v>0</v>
@@ -2756,7 +3011,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -2766,7 +3021,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -2776,7 +3031,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B71" s="6" t="n">
         <v>0</v>
@@ -2788,7 +3043,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B72" s="6" t="n">
         <v>0</v>
@@ -2800,7 +3055,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B73" s="6" t="n">
         <v>0</v>
@@ -2812,7 +3067,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B74" s="6" t="n">
         <v>0</v>
@@ -2824,7 +3079,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B75" s="6" t="n">
         <v>0</v>
@@ -2836,7 +3091,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B76" s="6" t="n">
         <v>0</v>
@@ -2865,7 +3120,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2886,55 +3141,55 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="n">
         <f aca="false">$B$2+ SUM($E4:$S4)</f>
@@ -2968,7 +3223,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="n">
         <f aca="false">SUM($E5:$S5)</f>
@@ -2998,12 +3253,12 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="n">
         <f aca="false">18+SUM(E8:S8)</f>
@@ -3019,7 +3274,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="n">
         <f aca="false">$B$4 + $C8</f>
@@ -3028,7 +3283,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="n">
         <f aca="false">$B$5 + $C8</f>
@@ -3037,7 +3292,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(0.5*$C8)</f>
@@ -3046,7 +3301,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(1.5*$C8)</f>
@@ -3072,7 +3327,7 @@
   <dimension ref="A1:AB20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3085,53 +3340,53 @@
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Z1" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" s="9" customFormat="true" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>1</v>
@@ -3190,7 +3445,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>0</v>
@@ -3259,7 +3514,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
         <f aca="false">'Salvador-Config'!$B$9</f>
@@ -3289,7 +3544,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="n">
         <f aca="false">'Salvador-Config'!$B$10</f>
@@ -3319,7 +3574,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>19</v>
@@ -3347,7 +3602,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>2</v>
@@ -3373,7 +3628,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>0</v>
@@ -3399,7 +3654,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="6"/>
       <c r="J10" s="6"/>
@@ -3410,7 +3665,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>0</v>
@@ -3436,7 +3691,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F12" s="6"/>
       <c r="J12" s="6" t="n">
@@ -3467,7 +3722,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="6"/>
       <c r="J13" s="6"/>
@@ -3483,7 +3738,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>0</v>
@@ -3509,7 +3764,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>0</v>
@@ -3535,7 +3790,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>0</v>
@@ -3561,7 +3816,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>0</v>
@@ -3587,7 +3842,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>0</v>
@@ -3613,7 +3868,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>0</v>
@@ -3663,8 +3918,8 @@
   </sheetPr>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3682,49 +3937,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="n">
         <f aca="false">$B$2+ SUM($E4:$S4)</f>
@@ -3749,7 +4004,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="n">
         <f aca="false">SUM($E5:$S5)</f>
@@ -3770,12 +4025,12 @@
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="n">
         <f aca="false">$B$11+$C$12+$B$13 + SUM($E8:$S8)</f>
@@ -3799,7 +4054,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(1.5*$C$12) + SUM($E9:$S9)</f>
@@ -3820,7 +4075,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>5</v>
@@ -3828,7 +4083,7 @@
     </row>
     <row r="12" s="10" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="10" t="n">
         <f aca="false">24 + SUM(E12:S12)</f>
@@ -3844,7 +4099,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>-1</v>
@@ -3852,12 +4107,12 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" s="10" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" s="10" t="n">
         <f aca="false">19 + SUM($E$16:$S$16)</f>
@@ -3873,7 +4128,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>-2</v>
@@ -3882,7 +4137,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="n">
         <f aca="false">$B$4 + $B17 + $C16</f>
@@ -3891,7 +4146,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="n">
         <f aca="false">$B$5 + $C16</f>
@@ -3900,7 +4155,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(0.5*$C16)</f>
@@ -3909,7 +4164,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(1.5*$C16)</f>
@@ -3918,12 +4173,12 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="n">
         <f aca="false">17 + SUM($E$16:$S$16)</f>
@@ -3936,7 +4191,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>-1</v>
@@ -3945,7 +4200,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="n">
         <f aca="false">$B$4 + $B25 + $C24</f>
@@ -3954,7 +4209,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B27" s="1" t="n">
         <f aca="false">$B$5 + $C24</f>
@@ -3963,7 +4218,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(0.5*$C24)</f>
@@ -3972,7 +4227,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B29" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(1.5*$C24)</f>
@@ -3981,12 +4236,12 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="n">
         <f aca="false">15 + SUM($E$16:$S$16)</f>
@@ -3999,7 +4254,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>0</v>
@@ -4008,7 +4263,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1" t="n">
         <f aca="false">$B$4 + $B33 + $C32</f>
@@ -4017,7 +4272,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" s="1" t="n">
         <f aca="false">$B$5 + $C32</f>
@@ -4026,7 +4281,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(0.5*$C32)</f>
@@ -4035,7 +4290,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(1.5*$C32)</f>
@@ -4061,7 +4316,7 @@
   <dimension ref="A1:R57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4073,47 +4328,47 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="47.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" s="4" customFormat="true" ht="36.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="N2" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>1</v>
@@ -4154,7 +4409,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>0</v>
@@ -4201,7 +4456,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$8</f>
@@ -4230,7 +4485,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$9</f>
@@ -4259,7 +4514,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>20</v>
@@ -4282,7 +4537,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>2</v>
@@ -4305,7 +4560,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>0</v>
@@ -4328,12 +4583,12 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>0</v>
@@ -4356,17 +4611,17 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>0</v>
@@ -4389,7 +4644,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>0</v>
@@ -4412,7 +4667,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>0</v>
@@ -4435,7 +4690,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>0</v>
@@ -4458,7 +4713,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>0</v>
@@ -4481,7 +4736,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>0</v>
@@ -4504,21 +4759,21 @@
     </row>
     <row r="21" s="4" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="Q21" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22" s="6" t="n">
         <v>2</v>
@@ -4547,7 +4802,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E23" s="6" t="n">
         <v>0</v>
@@ -4564,7 +4819,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E24" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$18</f>
@@ -4585,7 +4840,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E25" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$19*2</f>
@@ -4606,7 +4861,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E26" s="6" t="n">
         <v>20</v>
@@ -4623,7 +4878,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E27" s="6" t="n">
         <v>2</v>
@@ -4640,7 +4895,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E28" s="6" t="n">
         <v>0</v>
@@ -4657,12 +4912,12 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" s="6" t="n">
         <v>0</v>
@@ -4679,17 +4934,17 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E33" s="6" t="n">
         <v>0</v>
@@ -4706,7 +4961,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E34" s="6" t="n">
         <v>0</v>
@@ -4723,7 +4978,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E35" s="6" t="n">
         <v>0</v>
@@ -4740,7 +4995,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E36" s="6" t="n">
         <v>0</v>
@@ -4757,7 +5012,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E37" s="6" t="n">
         <v>0</v>
@@ -4774,7 +5029,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E38" s="6" t="n">
         <v>0</v>
@@ -4792,87 +5047,87 @@
     <row r="40" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -4894,10 +5149,10 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -4906,30 +5161,30 @@
     <row r="1" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F1" s="4"/>
     </row>
     <row r="2" s="5" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>1</v>
@@ -4949,7 +5204,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>0</v>
@@ -4961,7 +5216,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>12</v>
@@ -4973,7 +5228,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>10</v>
@@ -4985,7 +5240,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>20</v>
@@ -4997,7 +5252,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>2</v>
@@ -5009,7 +5264,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>0</v>
@@ -5021,7 +5276,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -5031,7 +5286,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>0</v>
@@ -5043,7 +5298,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -5053,7 +5308,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5063,7 +5318,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>0</v>
@@ -5075,7 +5330,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>0</v>
@@ -5087,7 +5342,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>0</v>
@@ -5099,7 +5354,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>0</v>
@@ -5111,7 +5366,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>0</v>
@@ -5123,7 +5378,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed bug that caused an error when the command line parameters -mi and -ma were used.
</commit_message>
<xml_diff>
--- a/input_test.xlsx
+++ b/input_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,6 +20,7 @@
     <sheet name="Tannenquelle-Config" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Tannenquelle" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Koboldstein" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Aliba Waffen" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="92">
   <si>
     <t xml:space="preserve">Testfälle</t>
   </si>
@@ -277,6 +278,36 @@
   </si>
   <si>
     <t xml:space="preserve">Krummsäbel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greatsword D+10 Auff.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falchion D+10 Sch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greatsword D+20 Auff.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falchion D+20 Sch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greatsword D+30 Auff.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falchion D+30 Sch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greatsword D+50 Auff.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falchion D+50 Sch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greatsword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falchion</t>
   </si>
 </sst>
 </file>
@@ -521,7 +552,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -594,7 +625,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -724,7 +755,7 @@
   <dimension ref="A1:AMJ59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1141,11 +1172,11 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="6" width="3.89"/>
@@ -1368,6 +1399,620 @@
         <v>25</v>
       </c>
       <c r="C37" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ59"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z6" activeCellId="0" sqref="Z6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="2" style="6" width="3.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="59" style="1" width="11.65"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="101.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AME1" s="1"/>
+      <c r="AMF1" s="1"/>
+      <c r="AMG1" s="1"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AME2" s="1"/>
+      <c r="AMF2" s="1"/>
+      <c r="AMG2" s="1"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="N3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="R3" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="T3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="U3" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="W3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="X3" s="6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>-5</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>-5</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6" t="n">
+        <v>-5</v>
+      </c>
+      <c r="N4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6" t="n">
+        <v>-5</v>
+      </c>
+      <c r="Q4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6" t="n">
+        <v>-5</v>
+      </c>
+      <c r="T4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="6" t="n">
+        <v>-5</v>
+      </c>
+      <c r="W4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="6" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <f aca="false">B6</f>
+        <v>23</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="K6" s="6" t="n">
+        <f aca="false">H6</f>
+        <v>24</v>
+      </c>
+      <c r="N6" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="6" t="n">
+        <f aca="false">N6</f>
+        <v>25</v>
+      </c>
+      <c r="T6" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="W6" s="6" t="n">
+        <f aca="false">T6</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="K7" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="N7" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="T7" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="W7" s="6" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="N8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="T8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="W8" s="6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="H12" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="N12" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="T12" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" s="6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AME21" s="1"/>
+      <c r="AMF21" s="1"/>
+      <c r="AMG21" s="1"/>
+      <c r="AMH21" s="0"/>
+      <c r="AMI21" s="0"/>
+      <c r="AMJ21" s="0"/>
+    </row>
+    <row r="40" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AME40" s="1"/>
+      <c r="AMF40" s="1"/>
+      <c r="AMG40" s="1"/>
+      <c r="AMH40" s="0"/>
+      <c r="AMI40" s="0"/>
+      <c r="AMJ40" s="0"/>
+    </row>
+    <row r="59" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AME59" s="1"/>
+      <c r="AMF59" s="1"/>
+      <c r="AMG59" s="1"/>
+      <c r="AMH59" s="0"/>
+      <c r="AMI59" s="0"/>
+      <c r="AMJ59" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1388,10 +2033,10 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -1788,10 +2433,10 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -2260,10 +2905,10 @@
   <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y42" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="Y42" activeCellId="0" sqref="Y42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -3120,7 +3765,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3327,7 +3972,7 @@
   <dimension ref="A1:AB20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3919,7 +4564,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4316,7 +4961,7 @@
   <dimension ref="A1:R57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5149,10 +5794,10 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>

</xml_diff>

<commit_message>
New calculations for Irgwi
</commit_message>
<xml_diff>
--- a/input_test.xlsx
+++ b/input_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,6 +21,7 @@
     <sheet name="Tannenquelle" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Koboldstein" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Aliba Waffen" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Irgwi-HA" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="93">
   <si>
     <t xml:space="preserve">Testfälle</t>
   </si>
@@ -308,6 +309,9 @@
   </si>
   <si>
     <t xml:space="preserve">Falchion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allo HA</t>
   </si>
 </sst>
 </file>
@@ -1418,15 +1422,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Z6" activeCellId="0" sqref="Z6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="2" style="6" width="3.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="59" style="1" width="11.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="59" style="1" width="11.64"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="101.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2013,6 +2017,556 @@
       <c r="AMH59" s="0"/>
       <c r="AMI59" s="0"/>
       <c r="AMJ59" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ57"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="2" style="6" width="3.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="54" style="1" width="11.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="ALZ1" s="0"/>
+      <c r="AMA1" s="0"/>
+      <c r="AMB1" s="0"/>
+      <c r="AMC1" s="0"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="36.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="ALZ2" s="0"/>
+      <c r="AMA2" s="0"/>
+      <c r="AMB2" s="0"/>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <f aca="false">IF(ISBLANK('Irgwi-Config'!$E$3), "", B4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <f aca="false">IF(ISBLANK('Irgwi-Config'!$E$3), "", E4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <f aca="false">'Irgwi-Config'!$B$18</f>
+        <v>11</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <f aca="false">$B5-2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <f aca="false">'Irgwi-Config'!$B$19</f>
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <f aca="false">$B6+4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" s="4" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="ALZ21" s="0"/>
+      <c r="AMA21" s="0"/>
+      <c r="AMB21" s="0"/>
+      <c r="AMC21" s="0"/>
+      <c r="AMD21" s="0"/>
+      <c r="AME21" s="0"/>
+      <c r="AMF21" s="0"/>
+      <c r="AMG21" s="0"/>
+      <c r="AMH21" s="0"/>
+      <c r="AMI21" s="0"/>
+      <c r="AMJ21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="6" t="n">
+        <f aca="false">'Irgwi-Config'!$B$18</f>
+        <v>11</v>
+      </c>
+      <c r="E24" s="6" t="n">
+        <f aca="false">$B24-2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="6" t="n">
+        <f aca="false">'Irgwi-Config'!$B$19*2</f>
+        <v>12</v>
+      </c>
+      <c r="E25" s="6" t="n">
+        <f aca="false">$B25+8</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E26" s="6" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="ALZ40" s="0"/>
+      <c r="AMA40" s="0"/>
+      <c r="AMB40" s="0"/>
+      <c r="AMC40" s="0"/>
+      <c r="AMD40" s="0"/>
+      <c r="AME40" s="0"/>
+      <c r="AMF40" s="0"/>
+      <c r="AMG40" s="0"/>
+      <c r="AMH40" s="0"/>
+      <c r="AMI40" s="0"/>
+      <c r="AMJ40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2036,7 +2590,7 @@
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -2436,7 +2990,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -2908,7 +3462,7 @@
       <selection pane="topLeft" activeCell="Y42" activeCellId="0" sqref="Y42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -4564,7 +5118,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4628,19 +5182,13 @@
       </c>
       <c r="B4" s="1" t="n">
         <f aca="false">$B$2+ SUM($E4:$S4)</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="8"/>
       <c r="E4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="H4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="J4" s="1" t="n">
@@ -4653,15 +5201,9 @@
       </c>
       <c r="B5" s="1" t="n">
         <f aca="false">SUM($E5:$S5)</f>
-        <v>5</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="J5" s="1" t="n">
@@ -4761,13 +5303,10 @@
       </c>
       <c r="B16" s="10" t="n">
         <f aca="false">19 + SUM($E$16:$S$16)</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C16" s="11" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(($B16-10)/2)</f>
-        <v>6</v>
-      </c>
-      <c r="L16" s="10" t="n">
         <v>4</v>
       </c>
     </row>
@@ -4786,7 +5325,7 @@
       </c>
       <c r="B18" s="1" t="n">
         <f aca="false">$B$4 + $B17 + $C16</f>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4795,7 +5334,7 @@
       </c>
       <c r="B19" s="1" t="n">
         <f aca="false">$B$5 + $C16</f>
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4804,7 +5343,7 @@
       </c>
       <c r="B20" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(0.5*$C16)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4813,7 +5352,7 @@
       </c>
       <c r="B21" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(1.5*$C16)</f>
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4827,11 +5366,11 @@
       </c>
       <c r="B24" s="1" t="n">
         <f aca="false">17 + SUM($E$16:$S$16)</f>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C24" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(($B24-10)/2)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4849,7 +5388,7 @@
       </c>
       <c r="B26" s="1" t="n">
         <f aca="false">$B$4 + $B25 + $C24</f>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4858,7 +5397,7 @@
       </c>
       <c r="B27" s="1" t="n">
         <f aca="false">$B$5 + $C24</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4867,7 +5406,7 @@
       </c>
       <c r="B28" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(0.5*$C24)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4876,7 +5415,7 @@
       </c>
       <c r="B29" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(1.5*$C24)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4890,11 +5429,11 @@
       </c>
       <c r="B32" s="1" t="n">
         <f aca="false">15 + SUM($E$16:$S$16)</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C32" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(($B32-10)/2)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4912,7 +5451,7 @@
       </c>
       <c r="B34" s="1" t="n">
         <f aca="false">$B$4 + $B33 + $C32</f>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4921,7 +5460,7 @@
       </c>
       <c r="B35" s="1" t="n">
         <f aca="false">$B$5 + $C32</f>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4930,7 +5469,7 @@
       </c>
       <c r="B36" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(0.5*$C32)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4939,7 +5478,7 @@
       </c>
       <c r="B37" s="1" t="n">
         <f aca="false">$B$5 + _xlfn.FLOOR.MATH(1.5*$C32)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -5109,23 +5648,23 @@
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$18</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H5" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$18</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="K5" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$26</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="N5" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$26</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Q5" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$34</f>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5138,23 +5677,23 @@
       </c>
       <c r="E6" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$19</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H6" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$19</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K6" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$27</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N6" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$29</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="Q6" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$35</f>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5468,19 +6007,19 @@
       </c>
       <c r="E24" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$18</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H24" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$18</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="K24" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$26</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Q24" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$34</f>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5489,19 +6028,19 @@
       </c>
       <c r="E25" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$19*2</f>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="H25" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$19</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K25" s="6" t="n">
         <f aca="false">2*'Irgwi-Config'!$B$27</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q25" s="6" t="n">
         <f aca="false">'Irgwi-Config'!$B$35</f>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5797,7 +6336,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>

</xml_diff>

<commit_message>
Added calculations for Aargan
</commit_message>
<xml_diff>
--- a/input_test.xlsx
+++ b/input_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,6 +22,7 @@
     <sheet name="Koboldstein" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Aliba Waffen" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Irgwi-HA" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Aargan" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="96">
   <si>
     <t xml:space="preserve">Testfälle</t>
   </si>
@@ -312,6 +313,15 @@
   </si>
   <si>
     <t xml:space="preserve">Allo HA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Std.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+2 Heilig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+1 Sch. Heilig</t>
   </si>
 </sst>
 </file>
@@ -1426,7 +1436,7 @@
       <selection pane="topLeft" activeCell="Z6" activeCellId="0" sqref="Z6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="2" style="6" width="3.89"/>
@@ -2036,7 +2046,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
     </sheetView>
   </sheetViews>
@@ -2568,6 +2578,319 @@
         <v>25</v>
       </c>
     </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O59"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="2" style="6" width="3.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="66" style="1" width="11.69"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="58.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="L3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="6" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>-10</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>-5</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>-10</v>
+      </c>
+      <c r="L4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6" t="n">
+        <v>-5</v>
+      </c>
+      <c r="O4" s="6" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="L6" s="6" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="L7" s="6" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="L8" s="6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L12" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="M12" s="6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2590,7 +2913,7 @@
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -2990,7 +3313,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -3462,7 +3785,7 @@
       <selection pane="topLeft" activeCell="Y42" activeCellId="0" sqref="Y42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>
@@ -6336,7 +6659,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="2" style="3" width="3.89"/>

</xml_diff>